<commit_message>
Add show_browser option to setup_driver and implement settings frame for user preferences
</commit_message>
<xml_diff>
--- a/data/excel_reports/shipments_2025-10-15.xlsx
+++ b/data/excel_reports/shipments_2025-10-15.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,182 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>240037217222</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>JESUSU ALBERTO HINCAPIE PJ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3173734168</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$ 267.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>240036364549</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pedro Antonio Gomez</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3043925139</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$ 37.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>240037128792</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>EDGAR BUITRAGO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3246465852</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$ 80.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>240037108787</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Martha Apolonia Galvis Portillo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3157200511</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$ 129.900,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>700170049543</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RINA ISABEL BERMUDEZ GUERRA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3226614162</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$ 45.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>700170495277</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RINA BERMUDEZ GUERRA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3226614162</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$ 45.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>240037036846</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Héctor Fabio Bastidas</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3152974198</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$ 94.900,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>240037080712</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Héctor Fabio Bastidas</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3152974198</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$ 100.000,00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add ProgressModal class for automation process feedback and enhance GuidesFrame with dynamic entry management
</commit_message>
<xml_diff>
--- a/data/excel_reports/shipments_2025-10-15.xlsx
+++ b/data/excel_reports/shipments_2025-10-15.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,6 +707,50 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>240037041835</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Michell Gabriela Tovar Ortega</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3137150103</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$ 130.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>240037041835</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Michell Gabriela Tovar Ortega</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3137150103</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$ 130.000,00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance login process with custom wait condition and improve error handling for authentication failures
</commit_message>
<xml_diff>
--- a/data/excel_reports/shipments_2025-10-15.xlsx
+++ b/data/excel_reports/shipments_2025-10-15.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,127 +512,127 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>240036846408</t>
+          <t>240037171791</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alex Aular</t>
+          <t>Kelly Johanna Perlaza Potes</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3158413931</t>
+          <t>3188658761</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$ 89.900,00</t>
+          <t>$ 48.999,00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>240037217222</t>
+          <t>700170507656</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>JESUSU ALBERTO HINCAPIE PJ</t>
+          <t>LEIDI PAOLA MARTINEZ</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3173734168</t>
+          <t>3176513277</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$ 267.000,00</t>
+          <t>$ 45.000,00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>240036364549</t>
+          <t>700170328932</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Pedro Antonio Gomez</t>
+          <t>XIMENA MUNOZ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3043925139</t>
+          <t>3184491249</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$ 37.000,00</t>
+          <t>$ 45.000,00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>240037128792</t>
+          <t>240037171791</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EDGAR BUITRAGO</t>
+          <t>Kelly Johanna Perlaza Potes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3246465852</t>
+          <t>3188658761</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$ 80.000,00</t>
+          <t>$ 48.999,00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>240037108787</t>
+          <t>700170507656</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Martha Apolonia Galvis Portillo</t>
+          <t>LEIDI PAOLA MARTINEZ</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3157200511</t>
+          <t>3176513277</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>$ 129.900,00</t>
+          <t>$ 45.000,00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>700170049543</t>
+          <t>700170328932</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RINA ISABEL BERMUDEZ GUERRA</t>
+          <t>XIMENA MUNOZ</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3226614162</t>
+          <t>3184491249</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -644,110 +644,264 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>700170495277</t>
+          <t>240037171791</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RINA BERMUDEZ GUERRA</t>
+          <t>Kelly Johanna Perlaza Potes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3226614162</t>
+          <t>3188658761</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>$ 45.000,00</t>
+          <t>$ 48.999,00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>240037036846</t>
+          <t>700170507656</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Héctor Fabio Bastidas</t>
+          <t>LEIDI PAOLA MARTINEZ</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3152974198</t>
+          <t>3176513277</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>$ 94.900,00</t>
+          <t>$ 45.000,00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>240037080712</t>
+          <t>240037171791</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Héctor Fabio Bastidas</t>
+          <t>Kelly Johanna Perlaza Potes</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3152974198</t>
+          <t>3188658761</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>$ 100.000,00</t>
+          <t>$ 48.999,00</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>240037041835</t>
+          <t>700170507656</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Michell Gabriela Tovar Ortega</t>
+          <t>LEIDI PAOLA MARTINEZ</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3137150103</t>
+          <t>3176513277</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>$ 130.000,00</t>
+          <t>$ 45.000,00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>240037041835</t>
+          <t>240037171791</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Michell Gabriela Tovar Ortega</t>
+          <t>Kelly Johanna Perlaza Potes</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3137150103</t>
+          <t>3188658761</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>$ 130.000,00</t>
+          <t>$ 48.999,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>700170507656</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>LEIDI PAOLA MARTINEZ</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3176513277</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$ 45.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>240037171791</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Kelly Johanna Perlaza Potes</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3188658761</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$ 48.999,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>700170507656</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>LEIDI PAOLA MARTINEZ</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3176513277</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$ 45.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>700170328932</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>XIMENA MUNOZ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3184491249</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$ 45.000,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>240036846408</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Alex Aular</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3158413931</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$ 89.900,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>240036846408</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Alex Aular</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3158413931</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$ 89.900,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>240037217222</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>JESUSU ALBERTO HINCAPIE PJ</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3173734168</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>$ 267.000,00</t>
         </is>
       </c>
     </row>

</xml_diff>